<commit_message>
Implemented soft constraint for the max altitude constraint
</commit_message>
<xml_diff>
--- a/src/Quadrotor_States.xlsx
+++ b/src/Quadrotor_States.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -428,1382 +428,2302 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>5.073169208943288</v>
+        <v>5.05256339220226</v>
       </c>
       <c r="B2">
-        <v>-0.028376439084989487</v>
+        <v>-0.05844122252062655</v>
       </c>
       <c r="C2">
-        <v>19.999999999671918</v>
+        <v>20.00143186137265</v>
       </c>
       <c r="D2">
-        <v>0.9641520738648012</v>
+        <v>0.9813605303747358</v>
       </c>
       <c r="E2">
-        <v>0.06792653252458915</v>
+        <v>0.14148139105040888</v>
       </c>
       <c r="F2">
-        <v>0.17490799515037161</v>
+        <v>0.1272251203673557</v>
       </c>
       <c r="G2">
-        <v>0.18611402649628273</v>
+        <v>0.024723616609225535</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>5.198658344166025</v>
+        <v>5.11076056248141</v>
       </c>
       <c r="B3">
-        <v>-0.07870355174395592</v>
+        <v>-0.06071164059579578</v>
       </c>
       <c r="C3">
-        <v>20.334042000471044</v>
+        <v>20.00107478390545</v>
       </c>
       <c r="D3">
-        <v>0.9502680686578826</v>
+        <v>0.9898582067425725</v>
       </c>
       <c r="E3">
-        <v>0.0939406172631884</v>
+        <v>0.005522851286703152</v>
       </c>
       <c r="F3">
-        <v>0.23422296209816884</v>
+        <v>0.14167441330103497</v>
       </c>
       <c r="G3">
-        <v>0.17961548499650404</v>
+        <v>-0.006930829388904424</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>5.943336874060615</v>
+        <v>5.1684783856700145</v>
       </c>
       <c r="B4">
-        <v>-0.07869014729786686</v>
+        <v>-0.08051854957723338</v>
       </c>
       <c r="C4">
-        <v>22.020586072909886</v>
+        <v>20.001671429779517</v>
       </c>
       <c r="D4">
-        <v>0.7316014844634704</v>
+        <v>0.984634327489087</v>
       </c>
       <c r="E4">
-        <v>-1.644299873210815e-5</v>
+        <v>0.04792520215181346</v>
       </c>
       <c r="F4">
-        <v>0.6671156440576403</v>
+        <v>0.1398652232141237</v>
       </c>
       <c r="G4">
-        <v>0.00015769815620508167</v>
+        <v>-0.09238854239295884</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
-        <v>5.943445852784647</v>
+        <v>5.226578176273162</v>
       </c>
       <c r="B5">
-        <v>-0.0761196544764599</v>
+        <v>-0.08105974170966172</v>
       </c>
       <c r="C5">
-        <v>21.399901073213243</v>
+        <v>20.000804308682152</v>
       </c>
       <c r="D5">
-        <v>0.9997895958520955</v>
+        <v>0.9899196759961719</v>
       </c>
       <c r="E5">
-        <v>-0.012732608036733643</v>
+        <v>0.0013188506606451298</v>
       </c>
       <c r="F5">
-        <v>0.0005383320043326232</v>
+        <v>0.1415178342017879</v>
       </c>
       <c r="G5">
-        <v>-0.016072805261726265</v>
+        <v>-0.0004791764466615682</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>6.605953988391703</v>
+        <v>5.2854450678618665</v>
       </c>
       <c r="B6">
-        <v>-0.07708738599640527</v>
+        <v>-0.07396125035796328</v>
       </c>
       <c r="C6">
-        <v>22.826904230480167</v>
+        <v>20.000080485149116</v>
       </c>
       <c r="D6">
-        <v>0.742956202931077</v>
+        <v>0.9888919381260376</v>
       </c>
       <c r="E6">
-        <v>0.000947909792751992</v>
+        <v>-0.017245956196137304</v>
       </c>
       <c r="F6">
-        <v>0.6555648412964232</v>
+        <v>0.14324940440950862</v>
       </c>
       <c r="G6">
-        <v>0.00037080118811202474</v>
+        <v>0.035085584126304734</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>6.620929810541013</v>
+        <v>5.3143356187040895</v>
       </c>
       <c r="B7">
-        <v>-0.07802112317101172</v>
+        <v>-0.07436331218336774</v>
       </c>
       <c r="C7">
-        <v>22.095637187802133</v>
+        <v>20.000192236432568</v>
       </c>
       <c r="D7">
-        <v>0.9958198633800064</v>
+        <v>0.9975152068822354</v>
       </c>
       <c r="E7">
-        <v>0.005653285604156249</v>
+        <v>0.0009793679428433543</v>
       </c>
       <c r="F7">
-        <v>0.09057438750583928</v>
+        <v>0.07059424828852673</v>
       </c>
       <c r="G7">
-        <v>0.01006037182621706</v>
+        <v>-4.006622040721618e-5</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>6.62095137974438</v>
+        <v>5.343365704338772</v>
       </c>
       <c r="B8">
-        <v>-0.07802165059766679</v>
+        <v>-0.07476728490600479</v>
       </c>
       <c r="C8">
-        <v>21.46479964659717</v>
+        <v>20.00019759333767</v>
       </c>
       <c r="D8">
-        <v>0.9999999698266734</v>
+        <v>0.9974907750022312</v>
       </c>
       <c r="E8">
-        <v>2.657278350088296e-6</v>
+        <v>0.0009840045285681989</v>
       </c>
       <c r="F8">
-        <v>0.00010867695199762693</v>
+        <v>0.07093982718296842</v>
       </c>
       <c r="G8">
-        <v>-0.000220292784355935</v>
+        <v>-4.057107292378602e-5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>6.62094772951908</v>
+        <v>5.291838821239579</v>
       </c>
       <c r="B9">
-        <v>-0.07802739342873574</v>
+        <v>-0.07542591637229533</v>
       </c>
       <c r="C9">
-        <v>20.908088871182812</v>
+        <v>20.000335027439597</v>
       </c>
       <c r="D9">
-        <v>0.9999999977443028</v>
+        <v>0.9920772578673986</v>
       </c>
       <c r="E9">
-        <v>2.5731872450664856e-5</v>
+        <v>0.0016045974096886406</v>
       </c>
       <c r="F9">
-        <v>-1.6355529308029378e-5</v>
+        <v>-0.1255463221385169</v>
       </c>
       <c r="G9">
-        <v>-5.9847821102519715e-5</v>
+        <v>8.062645461824147e-5</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>6.620948992549326</v>
+        <v>5.3501369979533955</v>
       </c>
       <c r="B10">
-        <v>-0.07802581597795043</v>
+        <v>-0.07544927369210747</v>
       </c>
       <c r="C10">
-        <v>20.38406101763481</v>
+        <v>20.000733752554407</v>
       </c>
       <c r="D10">
-        <v>0.9999999996229735</v>
+        <v>0.9898698828548463</v>
       </c>
       <c r="E10">
-        <v>-6.739109073588649e-6</v>
+        <v>5.678532436579376e-5</v>
       </c>
       <c r="F10">
-        <v>5.395858914814519e-6</v>
+        <v>0.14185778907201763</v>
       </c>
       <c r="G10">
-        <v>2.606764532329108e-5</v>
+        <v>-6.362162447042821e-5</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>6.650857601387378</v>
+        <v>5.408301406749585</v>
       </c>
       <c r="B11">
-        <v>-0.07858479165781462</v>
+        <v>-0.07566838488423157</v>
       </c>
       <c r="C11">
-        <v>20.000000000007947</v>
+        <v>20.000732340891766</v>
       </c>
       <c r="D11">
-        <v>0.9943333449780221</v>
+        <v>0.9899095689873284</v>
       </c>
       <c r="E11">
-        <v>0.001985172386539552</v>
+        <v>0.000532766495051208</v>
       </c>
       <c r="F11">
-        <v>0.1062371603926741</v>
+        <v>0.14158089241858893</v>
       </c>
       <c r="G11">
-        <v>-0.0005102228702385648</v>
+        <v>-0.0007477130675819267</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
-        <v>6.7022738542702776</v>
+        <v>5.466571961388493</v>
       </c>
       <c r="B12">
-        <v>-0.07948316577418925</v>
+        <v>-0.07589222356858445</v>
       </c>
       <c r="C12">
-        <v>19.999873806162753</v>
+        <v>20.00074804988271</v>
       </c>
       <c r="D12">
-        <v>0.9921065835343922</v>
+        <v>0.9898732753827215</v>
       </c>
       <c r="E12">
-        <v>0.0021894493145624212</v>
+        <v>0.0005445769561241475</v>
       </c>
       <c r="F12">
-        <v>0.12530574308879983</v>
+        <v>0.14183467231560068</v>
       </c>
       <c r="G12">
-        <v>0.00011105508890635248</v>
+        <v>-0.00033377065565802445</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13">
-        <v>6.753701682054283</v>
+        <v>5.525363663629996</v>
       </c>
       <c r="B13">
-        <v>-0.08038819742186024</v>
+        <v>-0.08240738038047872</v>
       </c>
       <c r="C13">
-        <v>19.999872672100853</v>
+        <v>20.0001140689421</v>
       </c>
       <c r="D13">
-        <v>0.9921044637202939</v>
+        <v>0.9890385101529628</v>
       </c>
       <c r="E13">
-        <v>0.002205463281369714</v>
+        <v>0.015829318388100706</v>
       </c>
       <c r="F13">
-        <v>0.12532156811905368</v>
+        <v>0.14307203455792467</v>
       </c>
       <c r="G13">
-        <v>0.00012148454833814864</v>
+        <v>-0.032253472255864696</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
-        <v>6.805127988945389</v>
+        <v>5.58380043877666</v>
       </c>
       <c r="B14">
-        <v>-0.0813010952500954</v>
+        <v>-0.08447006129884267</v>
       </c>
       <c r="C14">
-        <v>19.999828007160527</v>
+        <v>20.001098893667425</v>
       </c>
       <c r="D14">
-        <v>0.9921042994836654</v>
+        <v>0.9898029480410018</v>
       </c>
       <c r="E14">
-        <v>0.002224723980759183</v>
+        <v>0.005012848475338384</v>
       </c>
       <c r="F14">
-        <v>0.12532229576012144</v>
+        <v>0.14211792395828657</v>
       </c>
       <c r="G14">
-        <v>0.00014716669736429658</v>
+        <v>-0.006055400464256392</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
-        <v>6.856561518754301</v>
+        <v>5.642097338112591</v>
       </c>
       <c r="B15">
-        <v>-0.08219056016835105</v>
+        <v>-0.08363419439453906</v>
       </c>
       <c r="C15">
-        <v>19.999829073273542</v>
+        <v>20.00090522575166</v>
       </c>
       <c r="D15">
-        <v>0.9921028278475705</v>
+        <v>0.9898631385921257</v>
       </c>
       <c r="E15">
-        <v>0.0021673457351977965</v>
+        <v>-0.0020333734981008425</v>
       </c>
       <c r="F15">
-        <v>0.12533542553236257</v>
+        <v>0.14191516931318227</v>
       </c>
       <c r="G15">
-        <v>-0.0001312423920312786</v>
+        <v>0.00013667392940023377</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
-        <v>6.9087781352405075</v>
+        <v>5.70033364099307</v>
       </c>
       <c r="B16">
-        <v>-0.0831371053457009</v>
+        <v>-0.0841308562867962</v>
       </c>
       <c r="C16">
-        <v>19.999993569871055</v>
+        <v>20.000816268325767</v>
       </c>
       <c r="D16">
-        <v>0.9918632674106183</v>
+        <v>0.9898850934940449</v>
       </c>
       <c r="E16">
-        <v>0.0023060702285017014</v>
+        <v>0.0012099151311252524</v>
       </c>
       <c r="F16">
-        <v>0.12721132543872873</v>
+        <v>0.1417604383488843</v>
       </c>
       <c r="G16">
-        <v>0.00013519275420105294</v>
+        <v>-0.00026489879397713573</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17">
-        <v>6.961015935944239</v>
+        <v>5.7584543094192435</v>
       </c>
       <c r="B17">
-        <v>-0.08410634838243947</v>
+        <v>-0.08436028052698004</v>
       </c>
       <c r="C17">
-        <v>19.9999937439329</v>
+        <v>20.00072623932265</v>
       </c>
       <c r="D17">
-        <v>0.9918524776339191</v>
+        <v>0.9899233591202234</v>
       </c>
       <c r="E17">
-        <v>0.0023619431381781708</v>
+        <v>0.0005581938204134648</v>
       </c>
       <c r="F17">
-        <v>0.127278432478491</v>
+        <v>0.14148554893856416</v>
       </c>
       <c r="G17">
-        <v>0.0004810054430442985</v>
+        <v>-0.00038859720060776366</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18">
-        <v>7.013267674496656</v>
+        <v>5.7969343425026825</v>
       </c>
       <c r="B18">
-        <v>-0.08507650648213187</v>
+        <v>-0.08490905290123966</v>
       </c>
       <c r="C18">
-        <v>19.99999388469049</v>
+        <v>20.00023635187211</v>
       </c>
       <c r="D18">
-        <v>0.9918496196170441</v>
+        <v>0.9955727122277686</v>
       </c>
       <c r="E18">
-        <v>0.002364029640693305</v>
+        <v>0.00133972896642274</v>
       </c>
       <c r="F18">
-        <v>0.1273122122485526</v>
+        <v>0.09396144065292306</v>
       </c>
       <c r="G18">
-        <v>0.00025292456664089937</v>
+        <v>3.6366418054158317e-6</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19">
-        <v>7.065541245813937</v>
+        <v>5.826658704816033</v>
       </c>
       <c r="B19">
-        <v>-0.08605550337119149</v>
+        <v>-0.08535026066052014</v>
       </c>
       <c r="C19">
-        <v>19.999994025351825</v>
+        <v>20.00020572790846</v>
       </c>
       <c r="D19">
-        <v>0.991842814169707</v>
+        <v>0.9973691058616836</v>
       </c>
       <c r="E19">
-        <v>0.002385558142208298</v>
+        <v>0.0010747425341568052</v>
       </c>
       <c r="F19">
-        <v>0.12736498304881527</v>
+        <v>0.07263415977871976</v>
       </c>
       <c r="G19">
-        <v>0.00023664296954822536</v>
+        <v>-4.2686213924921896e-5</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20">
-        <v>7.1178380814820805</v>
+        <v>5.851114660649399</v>
       </c>
       <c r="B20">
-        <v>-0.08703815729327835</v>
+        <v>-0.08577688921553529</v>
       </c>
       <c r="C20">
-        <v>19.999994165945232</v>
+        <v>20.00014747065011</v>
       </c>
       <c r="D20">
-        <v>0.9918352087700034</v>
+        <v>0.9982216006181608</v>
       </c>
       <c r="E20">
-        <v>0.002394414533292411</v>
+        <v>0.0010388818232311436</v>
       </c>
       <c r="F20">
-        <v>0.12742128427459237</v>
+        <v>0.059786007815439315</v>
       </c>
       <c r="G20">
-        <v>0.0001854327824552207</v>
+        <v>2.2016698705789743e-6</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21">
-        <v>7.1701558129299485</v>
+        <v>5.882805685398091</v>
       </c>
       <c r="B21">
-        <v>-0.0880282323863342</v>
+        <v>-0.0862385551302805</v>
       </c>
       <c r="C21">
-        <v>19.999994306532077</v>
+        <v>20.00022204941989</v>
       </c>
       <c r="D21">
-        <v>0.9918291054348092</v>
+        <v>0.9970099208659771</v>
       </c>
       <c r="E21">
-        <v>0.0024124058739099937</v>
+        <v>0.001123950640681896</v>
       </c>
       <c r="F21">
-        <v>0.12747186813667233</v>
+        <v>0.07742098414733362</v>
       </c>
       <c r="G21">
-        <v>8.079764033125668e-5</v>
+        <v>-4.889961331892929e-5</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22">
-        <v>7.222486772232538</v>
+        <v>5.912982926575449</v>
       </c>
       <c r="B22">
-        <v>-0.08896500960502753</v>
+        <v>-0.0866861666409225</v>
       </c>
       <c r="C22">
-        <v>19.99999460698635</v>
+        <v>20.00020956888301</v>
       </c>
       <c r="D22">
-        <v>0.9918256238790332</v>
+        <v>0.9972883918363374</v>
       </c>
       <c r="E22">
-        <v>0.0022823814538260674</v>
+        <v>0.0010902177000794802</v>
       </c>
       <c r="F22">
-        <v>0.12750369230051523</v>
+        <v>0.07373706255941133</v>
       </c>
       <c r="G22">
-        <v>-0.0003594733125999042</v>
+        <v>-4.4087601270241705e-5</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23">
-        <v>7.274847947557471</v>
+        <v>5.861581212815967</v>
       </c>
       <c r="B23">
-        <v>-0.08997541550256773</v>
+        <v>-0.08742200780437767</v>
       </c>
       <c r="C23">
-        <v>19.999994583917683</v>
+        <v>20.0001751638801</v>
       </c>
       <c r="D23">
-        <v>0.9918156750507405</v>
+        <v>0.9921139309567493</v>
       </c>
       <c r="E23">
-        <v>0.002461961582380853</v>
+        <v>0.001791947391671434</v>
       </c>
       <c r="F23">
-        <v>0.1275768423031473</v>
+        <v>-0.12525979842956414</v>
       </c>
       <c r="G23">
-        <v>8.829093109727652e-5</v>
+        <v>0.0004020569674987747</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24">
-        <v>7.327229187199447</v>
+        <v>5.893321995617409</v>
       </c>
       <c r="B24">
-        <v>-0.09099120845261116</v>
+        <v>-0.08789246950747684</v>
       </c>
       <c r="C24">
-        <v>19.99999474478191</v>
+        <v>20.00022357954719</v>
       </c>
       <c r="D24">
-        <v>0.9918098654392251</v>
+        <v>0.9970003938422647</v>
       </c>
       <c r="E24">
-        <v>0.002475065488706703</v>
+        <v>0.0011454216386328246</v>
       </c>
       <c r="F24">
-        <v>0.1276253773744604</v>
+        <v>0.07754365694734629</v>
       </c>
       <c r="G24">
-        <v>5.3247102456864966e-5</v>
+        <v>-4.90687957961616e-5</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25">
-        <v>7.3796308514233235</v>
+        <v>5.925215361395892</v>
       </c>
       <c r="B25">
-        <v>-0.09198474787402258</v>
+        <v>-0.08836514976965812</v>
       </c>
       <c r="C25">
-        <v>19.999994942424046</v>
+        <v>20.000226940481916</v>
       </c>
       <c r="D25">
-        <v>0.9918038932657534</v>
+        <v>0.9969712998571322</v>
       </c>
       <c r="E25">
-        <v>0.0024205895946995027</v>
+        <v>0.0011507888610459186</v>
       </c>
       <c r="F25">
-        <v>0.12767480953822483</v>
+        <v>0.07791788523657432</v>
       </c>
       <c r="G25">
-        <v>-0.0003800054694214364</v>
+        <v>-4.960937447209101e-5</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26">
-        <v>7.432051036922695</v>
+        <v>5.957264156600536</v>
       </c>
       <c r="B26">
-        <v>-0.09299967083595834</v>
+        <v>-0.0888400883053766</v>
       </c>
       <c r="C26">
-        <v>19.999995080482222</v>
+        <v>20.000228693927234</v>
       </c>
       <c r="D26">
-        <v>0.9917983416810892</v>
+        <v>0.9969417052335487</v>
       </c>
       <c r="E26">
-        <v>0.002472932639070523</v>
+        <v>0.001156242348637936</v>
       </c>
       <c r="F26">
-        <v>0.1277195239028236</v>
+        <v>0.07829661391739091</v>
       </c>
       <c r="G26">
-        <v>-1.9727778522785202e-5</v>
+        <v>-5.012518414071884e-5</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27">
-        <v>7.484491486884473</v>
+        <v>5.9894689859710315</v>
       </c>
       <c r="B27">
-        <v>-0.09402147723209449</v>
+        <v>-0.08931729320841619</v>
       </c>
       <c r="C27">
-        <v>19.99999521842797</v>
+        <v>20.000230405514404</v>
       </c>
       <c r="D27">
-        <v>0.991792191235954</v>
+        <v>0.9969118578490196</v>
       </c>
       <c r="E27">
-        <v>0.0024897139381055435</v>
+        <v>0.0011617144838369914</v>
       </c>
       <c r="F27">
-        <v>0.12776854219364722</v>
+        <v>0.07867671202841886</v>
       </c>
       <c r="G27">
-        <v>2.204598334703444e-5</v>
+        <v>-5.0643844935645955e-5</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
-        <v>7.536961225074725</v>
+        <v>6.021830371563342</v>
       </c>
       <c r="B28">
-        <v>-0.0950630420781558</v>
+        <v>-0.08979677139661732</v>
       </c>
       <c r="C28">
-        <v>19.999995486454623</v>
+        <v>20.000232131788</v>
       </c>
       <c r="D28">
-        <v>0.9917799779323434</v>
+        <v>0.9968817656261437</v>
       </c>
       <c r="E28">
-        <v>0.002537816028261589</v>
+        <v>0.0011672027367477529</v>
       </c>
       <c r="F28">
-        <v>0.12783874560908964</v>
+        <v>0.07905806227526865</v>
       </c>
       <c r="G28">
-        <v>-0.00011487276669762343</v>
+        <v>-5.1166361313906966e-5</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29">
-        <v>7.589453918351046</v>
+        <v>6.054348830812312</v>
       </c>
       <c r="B29">
-        <v>-0.09611228745124877</v>
+        <v>-0.09027852971249817</v>
       </c>
       <c r="C29">
-        <v>19.99999557887262</v>
+        <v>20.000233874912762</v>
       </c>
       <c r="D29">
-        <v>0.9917739364415004</v>
+        <v>0.9968514277812222</v>
       </c>
       <c r="E29">
-        <v>0.0025563615680153622</v>
+        <v>0.0011727069296640553</v>
       </c>
       <c r="F29">
-        <v>0.1278944392024643</v>
+        <v>0.0794406562101629</v>
       </c>
       <c r="G29">
-        <v>-0.00033899453020985276</v>
+        <v>-5.169277534842531e-5</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30">
-        <v>7.641965173282231</v>
+        <v>6.085336245689358</v>
       </c>
       <c r="B30">
-        <v>-0.0971706620532481</v>
+        <v>-0.09074654901060815</v>
       </c>
       <c r="C30">
-        <v>19.999995890765888</v>
+        <v>20.000218021308118</v>
       </c>
       <c r="D30">
-        <v>0.9917677406347453</v>
+        <v>0.997140804656919</v>
       </c>
       <c r="E30">
-        <v>0.0025787094723443964</v>
+        <v>0.0011397673295638134</v>
       </c>
       <c r="F30">
-        <v>0.12793919984185567</v>
+        <v>0.0757116453463124</v>
       </c>
       <c r="G30">
-        <v>-0.00015576574594962977</v>
+        <v>-4.665349353956287e-5</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31">
-        <v>7.694495579884945</v>
+        <v>6.1181631669564105</v>
       </c>
       <c r="B31">
-        <v>-0.09823893183566088</v>
+        <v>-0.09123283119173205</v>
       </c>
       <c r="C31">
-        <v>19.999996061086208</v>
+        <v>20.000236688709105</v>
       </c>
       <c r="D31">
-        <v>0.9917620581766965</v>
+        <v>0.9967914992816519</v>
       </c>
       <c r="E31">
-        <v>0.0026029425715320964</v>
+        <v>0.0011836235186213635</v>
       </c>
       <c r="F31">
-        <v>0.12798554015820252</v>
+        <v>0.08019097501092047</v>
       </c>
       <c r="G31">
-        <v>-1.462098944237934e-5</v>
+        <v>-5.2718180835901076e-5</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32">
-        <v>7.747048345234885</v>
+        <v>6.143341003839844</v>
       </c>
       <c r="B32">
-        <v>-0.09932026507269277</v>
+        <v>-0.09168922704343238</v>
       </c>
       <c r="C32">
-        <v>19.999996192452898</v>
+        <v>20.00015366327127</v>
       </c>
       <c r="D32">
-        <v>0.9917559656233175</v>
+        <v>0.9981148127245377</v>
       </c>
       <c r="E32">
-        <v>0.002634811931328362</v>
+        <v>0.0011113246007057106</v>
       </c>
       <c r="F32">
-        <v>0.12803971235069236</v>
+        <v>0.06154885451038006</v>
       </c>
       <c r="G32">
-        <v>2.5281688417376047e-5</v>
+        <v>2.4911410207325326e-6</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33">
-        <v>7.799632274938338</v>
+        <v>6.106873300528015</v>
       </c>
       <c r="B33">
-        <v>-0.1004481408345602</v>
+        <v>-0.09247406084633998</v>
       </c>
       <c r="C33">
-        <v>19.9999959746243</v>
+        <v>20.000201354898685</v>
       </c>
       <c r="D33">
-        <v>0.9917459763687968</v>
+        <v>0.9960248563666421</v>
       </c>
       <c r="E33">
-        <v>0.0027482154037956528</v>
+        <v>0.0019161708191343283</v>
       </c>
       <c r="F33">
-        <v>0.1281148730609796</v>
+        <v>-0.08903529909198835</v>
       </c>
       <c r="G33">
-        <v>9.794683406554074e-5</v>
+        <v>4.888287996912392e-6</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34">
-        <v>7.852238111532764</v>
+        <v>6.142598365232279</v>
       </c>
       <c r="B34">
-        <v>-0.101590370789074</v>
+        <v>-0.09301529084320544</v>
       </c>
       <c r="C34">
-        <v>19.999996114624764</v>
+        <v>20.000196324337566</v>
       </c>
       <c r="D34">
-        <v>0.9917393304276243</v>
+        <v>0.9961856779373339</v>
       </c>
       <c r="E34">
-        <v>0.002783376132726939</v>
+        <v>0.001321288996765934</v>
       </c>
       <c r="F34">
-        <v>0.12816766617499767</v>
+        <v>0.08723269848816681</v>
       </c>
       <c r="G34">
-        <v>0.0001799720863674096</v>
+        <v>3.152009384111711e-6</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35">
-        <v>7.904874333360549</v>
+        <v>6.178511168157083</v>
       </c>
       <c r="B35">
-        <v>-0.10277971548683859</v>
+        <v>-0.09355936882607901</v>
       </c>
       <c r="C35">
-        <v>19.99999630909253</v>
+        <v>20.000197737409064</v>
       </c>
       <c r="D35">
-        <v>0.9917280782632988</v>
+        <v>0.9961455623931134</v>
       </c>
       <c r="E35">
-        <v>0.002898189353018462</v>
+        <v>0.0013282067255424076</v>
       </c>
       <c r="F35">
-        <v>0.12823996354948874</v>
+        <v>0.08768895563085438</v>
       </c>
       <c r="G35">
-        <v>0.00022505536902893056</v>
+        <v>3.179886703514076e-6</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36">
-        <v>8.143961499971214</v>
+        <v>6.216435763569733</v>
       </c>
       <c r="B36">
-        <v>-0.1712901965800958</v>
+        <v>-0.09420056651458276</v>
       </c>
       <c r="C36">
-        <v>20.42257162456889</v>
+        <v>20.000215268118385</v>
       </c>
       <c r="D36">
-        <v>0.8781310394331879</v>
+        <v>0.9957020447261691</v>
       </c>
       <c r="E36">
-        <v>0.11539627625029718</v>
+        <v>0.0015649402543437385</v>
       </c>
       <c r="F36">
-        <v>0.40649889091571545</v>
+        <v>0.09257944044210205</v>
       </c>
       <c r="G36">
-        <v>0.2117840264339755</v>
+        <v>3.492754143200163e-6</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37">
-        <v>8.172204261022326</v>
+        <v>6.252734097387901</v>
       </c>
       <c r="B37">
-        <v>-0.17240854000375502</v>
+        <v>-0.09475088182573099</v>
       </c>
       <c r="C37">
-        <v>19.999999999999993</v>
+        <v>20.00020155963685</v>
       </c>
       <c r="D37">
-        <v>0.9944429286387118</v>
+        <v>0.9960623758141159</v>
       </c>
       <c r="E37">
-        <v>0.00416189260796063</v>
+        <v>0.0013433886630861366</v>
       </c>
       <c r="F37">
-        <v>0.10513286477179366</v>
+        <v>0.08862749708580087</v>
       </c>
       <c r="G37">
-        <v>-0.001661874369205379</v>
+        <v>3.240672104392183e-6</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38">
-        <v>8.22494388056763</v>
+        <v>6.284552461775739</v>
       </c>
       <c r="B38">
-        <v>-0.17420987611031719</v>
+        <v>-0.09525898102526405</v>
       </c>
       <c r="C38">
-        <v>19.99999642964262</v>
+        <v>20.00022535765848</v>
       </c>
       <c r="D38">
-        <v>0.991693637694984</v>
+        <v>0.9969855047195458</v>
       </c>
       <c r="E38">
-        <v>0.004388128694210878</v>
+        <v>0.0012373348453792465</v>
       </c>
       <c r="F38">
-        <v>0.12849188604297881</v>
+        <v>0.07773402654590664</v>
       </c>
       <c r="G38">
-        <v>-4.416718855647947e-5</v>
+        <v>-4.927098321263245e-5</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39">
-        <v>8.27648078148682</v>
+        <v>6.309861389195119</v>
       </c>
       <c r="B39">
-        <v>-0.17674205055619854</v>
+        <v>-0.0958468805714878</v>
       </c>
       <c r="C39">
-        <v>19.999742991855815</v>
+        <v>20.00015427062856</v>
       </c>
       <c r="D39">
-        <v>0.9920539965532629</v>
+        <v>0.9980947372632161</v>
       </c>
       <c r="E39">
-        <v>0.006172388707575695</v>
+        <v>0.0014326922696968857</v>
       </c>
       <c r="F39">
-        <v>0.125609586371057</v>
+        <v>0.06186823192666134</v>
       </c>
       <c r="G39">
-        <v>0.0002963147613074188</v>
+        <v>3.32494187778376e-6</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40">
-        <v>8.329290489552356</v>
+        <v>6.342091766570134</v>
       </c>
       <c r="B40">
-        <v>-0.17862988255536463</v>
+        <v>-0.09636019892408589</v>
       </c>
       <c r="C40">
-        <v>19.99999669770926</v>
+        <v>20.000227958173085</v>
       </c>
       <c r="D40">
-        <v>0.9916728750597834</v>
+        <v>0.9969071605069367</v>
       </c>
       <c r="E40">
-        <v>0.004598300787874255</v>
+        <v>0.0012498987134190033</v>
       </c>
       <c r="F40">
-        <v>0.1286354050314609</v>
+        <v>0.07873487317440891</v>
       </c>
       <c r="G40">
-        <v>-0.0001911733017124957</v>
+        <v>-5.059368860630765e-5</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41">
-        <v>8.380777212858765</v>
+        <v>6.372306932766875</v>
       </c>
       <c r="B41">
-        <v>-0.18058957673213036</v>
+        <v>-0.09691978577483235</v>
       </c>
       <c r="C41">
-        <v>19.999762688366346</v>
+        <v>20.000210170994226</v>
       </c>
       <c r="D41">
-        <v>0.9920753319450301</v>
+        <v>0.9972812168928595</v>
       </c>
       <c r="E41">
-        <v>0.004776492554199017</v>
+        <v>0.001363781543137576</v>
       </c>
       <c r="F41">
-        <v>0.12548600042788008</v>
+        <v>0.07382976791509825</v>
       </c>
       <c r="G41">
-        <v>-4.447363707939665e-5</v>
+        <v>-4.401096118046319e-5</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42">
-        <v>8.432285392323742</v>
+        <v>6.409416504504535</v>
       </c>
       <c r="B42">
-        <v>-0.18257282977823508</v>
+        <v>-0.09748449049873344</v>
       </c>
       <c r="C42">
-        <v>19.999760471237405</v>
+        <v>20.000208397371914</v>
       </c>
       <c r="D42">
-        <v>0.9920712383087392</v>
+        <v>0.9958846805657448</v>
       </c>
       <c r="E42">
-        <v>0.004832915646351225</v>
+        <v>0.0013783724605744626</v>
       </c>
       <c r="F42">
-        <v>0.12551618913166784</v>
+        <v>0.09059938785839647</v>
       </c>
       <c r="G42">
-        <v>-0.00013771983884487164</v>
+        <v>3.3642584357824156e-6</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43">
-        <v>8.483798215902876</v>
+        <v>6.44671826869409</v>
       </c>
       <c r="B43">
-        <v>-0.18456319152897613</v>
+        <v>-0.09807122915286663</v>
       </c>
       <c r="C43">
-        <v>19.99975902892298</v>
+        <v>20.00021003367004</v>
       </c>
       <c r="D43">
-        <v>0.9920697057098343</v>
+        <v>0.995841949834811</v>
       </c>
       <c r="E43">
-        <v>0.004850134057622919</v>
+        <v>0.0014321278912134848</v>
       </c>
       <c r="F43">
-        <v>0.125527322799103</v>
+        <v>0.09106643186426167</v>
       </c>
       <c r="G43">
-        <v>-0.0003059459079664804</v>
+        <v>3.3948691377535913e-6</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44">
-        <v>8.53531889969012</v>
+        <v>6.484212697493496</v>
       </c>
       <c r="B44">
-        <v>-0.1855204780626318</v>
+        <v>-0.09864190961260594</v>
       </c>
       <c r="C44">
-        <v>19.999744422778434</v>
+        <v>20.0002117843202</v>
       </c>
       <c r="D44">
-        <v>0.9920780148345304</v>
+        <v>0.9957990069971517</v>
       </c>
       <c r="E44">
-        <v>0.002333386383039847</v>
+        <v>0.0013928909180425393</v>
       </c>
       <c r="F44">
-        <v>0.12554836565939642</v>
+        <v>0.09153480005465599</v>
       </c>
       <c r="G44">
-        <v>0.0007240908921248426</v>
+        <v>3.423414632746235e-6</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45">
-        <v>8.586840675691139</v>
+        <v>6.519904212388029</v>
       </c>
       <c r="B45">
-        <v>-0.18757506281766012</v>
+        <v>-0.09929379798055225</v>
       </c>
       <c r="C45">
-        <v>19.99975148643452</v>
+        <v>20.000196376382934</v>
       </c>
       <c r="D45">
-        <v>0.9920658979938402</v>
+        <v>0.9961923814497954</v>
       </c>
       <c r="E45">
-        <v>0.005006541097836983</v>
+        <v>0.0015915084005453189</v>
       </c>
       <c r="F45">
-        <v>0.12554814468752734</v>
+        <v>0.087151684167821</v>
       </c>
       <c r="G45">
-        <v>-0.00040851237392358695</v>
+        <v>3.1552279910507113e-6</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46">
-        <v>8.668679999849376</v>
+        <v>6.55164312128634</v>
       </c>
       <c r="B46">
-        <v>-0.1886882327919863</v>
+        <v>-0.09986298444877201</v>
       </c>
       <c r="C46">
-        <v>20.116487155827784</v>
+        <v>20.000224351740442</v>
       </c>
       <c r="D46">
-        <v>0.9656523405192579</v>
+        <v>0.9970003566358964</v>
       </c>
       <c r="E46">
-        <v>0.002524298558454595</v>
+        <v>0.0013865884845313484</v>
       </c>
       <c r="F46">
-        <v>0.17878512950479028</v>
+        <v>0.07754022112284419</v>
       </c>
       <c r="G46">
-        <v>0.18715055943655393</v>
+        <v>-4.8881530320527376e-5</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47">
-        <v>9.458440460302112</v>
+        <v>6.587841143268808</v>
       </c>
       <c r="B47">
-        <v>-0.19025468242081192</v>
+        <v>-0.1004262645463536</v>
       </c>
       <c r="C47">
-        <v>21.926019987829562</v>
+        <v>20.000200986340797</v>
       </c>
       <c r="D47">
-        <v>0.722924363547155</v>
+        <v>0.9960839847931537</v>
       </c>
       <c r="E47">
-        <v>0.0013755249325182932</v>
+        <v>0.0013750703341203635</v>
       </c>
       <c r="F47">
-        <v>0.6756579387635101</v>
+        <v>0.08838411303596735</v>
       </c>
       <c r="G47">
-        <v>-0.0011917394875567875</v>
+        <v>3.2273831868516323e-6</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48">
-        <v>9.459743009273843</v>
+        <v>6.62606161681383</v>
       </c>
       <c r="B48">
-        <v>-0.1922916795647771</v>
+        <v>-0.1010263330188222</v>
       </c>
       <c r="C48">
-        <v>21.318432621024883</v>
+        <v>20.000218041633946</v>
       </c>
       <c r="D48">
-        <v>0.9993726513736269</v>
+        <v>0.9956349776235057</v>
       </c>
       <c r="E48">
-        <v>0.00987156288456035</v>
+        <v>0.001464484249394706</v>
       </c>
       <c r="F48">
-        <v>0.006315664815935785</v>
+        <v>0.09329859102266158</v>
       </c>
       <c r="G48">
-        <v>-0.03341883531417179</v>
+        <v>3.5357402121262228e-6</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49">
-        <v>9.45974139393566</v>
+        <v>6.66447691129823</v>
       </c>
       <c r="B49">
-        <v>-0.1923137284595929</v>
+        <v>-0.10170827628716343</v>
       </c>
       <c r="C49">
-        <v>20.77028520091881</v>
+        <v>20.000220352768313</v>
       </c>
       <c r="D49">
-        <v>0.9999999941177816</v>
+        <v>0.9955900339463154</v>
       </c>
       <c r="E49">
-        <v>9.754672013807153e-5</v>
+        <v>0.0016643209628002225</v>
       </c>
       <c r="F49">
-        <v>-7.14646595805019e-6</v>
+        <v>0.09377296751502995</v>
       </c>
       <c r="G49">
-        <v>4.6882854298664006e-5</v>
+        <v>3.5736384127551277e-6</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50">
-        <v>9.459751415912214</v>
+        <v>6.704713394493513</v>
       </c>
       <c r="B50">
-        <v>-0.1923095392719592</v>
+        <v>-0.10238856643294772</v>
       </c>
       <c r="C50">
-        <v>20.254353186796727</v>
+        <v>20.00026423213105</v>
       </c>
       <c r="D50">
-        <v>0.9824212773636702</v>
+        <v>0.9951625788504987</v>
       </c>
       <c r="E50">
-        <v>-1.740791810587814e-5</v>
+        <v>0.0016601217995656295</v>
       </c>
       <c r="F50">
-        <v>4.176565605665657e-5</v>
+        <v>0.09819420006888686</v>
       </c>
       <c r="G50">
-        <v>0.18640449301018772</v>
+        <v>8.135395831997807e-7</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51">
-        <v>9.520359633830271</v>
+        <v>6.737146401626442</v>
       </c>
       <c r="B51">
-        <v>-0.20160660818874002</v>
+        <v>-0.10293104309438864</v>
       </c>
       <c r="C51">
-        <v>20.00001641171317</v>
+        <v>20.00023414461768</v>
       </c>
       <c r="D51">
-        <v>0.9646648262130849</v>
+        <v>0.9968676229559159</v>
       </c>
       <c r="E51">
-        <v>0.027964277759683243</v>
+        <v>0.0013210665488337064</v>
       </c>
       <c r="F51">
-        <v>0.18288882138686977</v>
+        <v>0.07923432203201955</v>
       </c>
       <c r="G51">
-        <v>-0.18612275050109175</v>
+        <v>-5.1302356602197225e-5</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52">
-        <v>9.57195977242744</v>
+        <v>6.776127190590343</v>
       </c>
       <c r="B52">
-        <v>-0.20366657156214593</v>
+        <v>-0.10352692112111417</v>
       </c>
       <c r="C52">
-        <v>19.999725361387476</v>
+        <v>20.00022607094331</v>
       </c>
       <c r="D52">
-        <v>0.9920408951784125</v>
+        <v>0.9954597304042928</v>
       </c>
       <c r="E52">
-        <v>0.005021153270827973</v>
+        <v>0.0014541397558529487</v>
       </c>
       <c r="F52">
-        <v>0.12576619601983732</v>
+        <v>0.09514776193629494</v>
       </c>
       <c r="G52">
-        <v>-0.00036250578787724934</v>
+        <v>3.656819062932192e-6</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53">
-        <v>9.653770718971106</v>
+        <v>6.813499138198775</v>
       </c>
       <c r="B53">
-        <v>-0.20881921234433945</v>
+        <v>-0.10412731256097921</v>
       </c>
       <c r="C53">
-        <v>20.12154378135186</v>
+        <v>20.0002111901647</v>
       </c>
       <c r="D53">
-        <v>0.9657369554724325</v>
+        <v>0.9958261697713798</v>
       </c>
       <c r="E53">
-        <v>0.011307042383526587</v>
+        <v>0.0014654637951902211</v>
       </c>
       <c r="F53">
-        <v>0.17805286127247008</v>
+        <v>0.09123806550399388</v>
       </c>
       <c r="G53">
-        <v>0.18709427973280493</v>
+        <v>3.408618473867968e-6</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54">
-        <v>9.69963069645066</v>
+        <v>6.852868762751613</v>
       </c>
       <c r="B54">
-        <v>-0.2106063026950142</v>
+        <v>-0.10491974875827621</v>
       </c>
       <c r="C54">
-        <v>20.000000000000004</v>
+        <v>20.00022907322212</v>
       </c>
       <c r="D54">
-        <v>0.9922452447419549</v>
+        <v>0.9953681997987612</v>
       </c>
       <c r="E54">
-        <v>0.0048313546613357825</v>
+        <v>0.0019337794534182518</v>
       </c>
       <c r="F54">
-        <v>0.12405719983438213</v>
+        <v>0.09609073729600341</v>
       </c>
       <c r="G54">
-        <v>-0.003983978501520832</v>
+        <v>3.728700903792367e-6</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55">
-        <v>9.75124882805125</v>
+        <v>6.8907017360673235</v>
       </c>
       <c r="B55">
-        <v>-0.21281129721756364</v>
+        <v>-0.10564177298525886</v>
       </c>
       <c r="C55">
-        <v>19.99972012425782</v>
+        <v>20.00021540690742</v>
       </c>
       <c r="D55">
-        <v>0.9920333554121044</v>
+        <v>0.995722243844625</v>
       </c>
       <c r="E55">
-        <v>0.005375120569548828</v>
+        <v>0.001762307812997961</v>
       </c>
       <c r="F55">
-        <v>0.12580886127315527</v>
+        <v>0.09235866821820823</v>
       </c>
       <c r="G55">
-        <v>0.00027657238409848695</v>
+        <v>3.4880913184940923e-6</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56">
-        <v>9.802891180800264</v>
+        <v>6.935417857859401</v>
       </c>
       <c r="B56">
-        <v>-0.21503787876186617</v>
+        <v>-0.10661684039072696</v>
       </c>
       <c r="C56">
-        <v>19.99972480453675</v>
+        <v>20.000423791548624</v>
       </c>
       <c r="D56">
-        <v>0.9920292585995034</v>
+        <v>0.9940274622858977</v>
       </c>
       <c r="E56">
-        <v>0.0054258830141443405</v>
+        <v>0.0023779020504573942</v>
       </c>
       <c r="F56">
-        <v>0.12584120323885406</v>
+        <v>0.10905075139170622</v>
       </c>
       <c r="G56">
-        <v>0.0005983189092041703</v>
+        <v>1.2832505636802233e-6</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57">
-        <v>9.854540190995081</v>
+        <v>6.963898151144365</v>
       </c>
       <c r="B57">
-        <v>-0.21731499241157032</v>
+        <v>-0.10718838022716844</v>
       </c>
       <c r="C57">
-        <v>19.999723260084707</v>
+        <v>20.00020102155008</v>
       </c>
       <c r="D57">
-        <v>0.992026193530801</v>
+        <v>0.9975836666681517</v>
       </c>
       <c r="E57">
-        <v>0.005549692974793455</v>
+        <v>0.0013937470676639715</v>
       </c>
       <c r="F57">
-        <v>0.12585745413149704</v>
+        <v>0.06961077479225919</v>
       </c>
       <c r="G57">
-        <v>0.00040674381353621755</v>
+        <v>-3.88077878879416e-5</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58">
-        <v>9.906196601794072</v>
+        <v>7.000414853001457</v>
       </c>
       <c r="B58">
-        <v>-0.21963822953434822</v>
+        <v>-0.10781328109851934</v>
       </c>
       <c r="C58">
-        <v>19.99972179471787</v>
+        <v>20.000202999554027</v>
       </c>
       <c r="D58">
-        <v>0.992022948133181</v>
+        <v>0.9960147465981349</v>
       </c>
       <c r="E58">
-        <v>0.005662120503586323</v>
+        <v>0.0015254405247067755</v>
       </c>
       <c r="F58">
-        <v>0.12587522501977663</v>
+        <v>0.08915758396970219</v>
       </c>
       <c r="G58">
-        <v>0.00016578527486941857</v>
+        <v>3.277033070214492e-6</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59">
-        <v>9.957860277609079</v>
+        <v>7.040545827539268</v>
       </c>
       <c r="B59">
-        <v>-0.22200069952460572</v>
+        <v>-0.10862107978281026</v>
       </c>
       <c r="C59">
-        <v>19.999720324033927</v>
+        <v>20.000262524742055</v>
       </c>
       <c r="D59">
-        <v>0.992019830483543</v>
+        <v>0.9951874067391052</v>
       </c>
       <c r="E59">
-        <v>0.005757609027827989</v>
+        <v>0.0019712988809204753</v>
       </c>
       <c r="F59">
-        <v>0.12589272717645125</v>
+        <v>0.09793688524063807</v>
       </c>
       <c r="G59">
-        <v>-7.754546158723701e-5</v>
+        <v>8.071768157896646e-7</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60">
-        <v>10.029018349568656</v>
+        <v>7.071210772289519</v>
       </c>
       <c r="B60">
-        <v>-0.24421007854940846</v>
+        <v>-0.10920149594812238</v>
       </c>
       <c r="C60">
-        <v>19.987911511994728</v>
+        <v>20.000215861472206</v>
       </c>
       <c r="D60">
-        <v>0.965604384065906</v>
+        <v>0.9971995167347256</v>
       </c>
       <c r="E60">
-        <v>0.053749745680964925</v>
+        <v>0.001414500561756713</v>
       </c>
       <c r="F60">
-        <v>0.1719038552134231</v>
+        <v>0.07492747916392299</v>
       </c>
       <c r="G60">
-        <v>0.18613681297530507</v>
+        <v>-4.5426963327733266e-5</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61">
-        <v>10.083543967443958</v>
+        <v>7.10942899541342</v>
       </c>
       <c r="B61">
-        <v>-0.24693568048547584</v>
+        <v>-0.11001884382081284</v>
       </c>
       <c r="C61">
-        <v>19.99967541794583</v>
+        <v>20.00021850884793</v>
       </c>
       <c r="D61">
-        <v>0.9912802410273951</v>
+        <v>0.99563448673663</v>
       </c>
       <c r="E61">
-        <v>0.006577423558375139</v>
+        <v>0.001994893279315311</v>
       </c>
       <c r="F61">
-        <v>0.13155180007189768</v>
+        <v>0.09329398433445579</v>
       </c>
       <c r="G61">
-        <v>0.0006235130136186967</v>
+        <v>3.5526212645847277e-6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62">
+        <v>7.149912101077057</v>
+      </c>
+      <c r="B62">
+        <v>-0.11064561622312118</v>
+      </c>
+      <c r="C62">
+        <v>20.00035791149437</v>
+      </c>
+      <c r="D62">
+        <v>0.995103566183205</v>
+      </c>
+      <c r="E62">
+        <v>0.0015294194120025544</v>
+      </c>
+      <c r="F62">
+        <v>0.09878630174068366</v>
+      </c>
+      <c r="G62">
+        <v>1.0470204599140672e-6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63">
+        <v>7.181095114204883</v>
+      </c>
+      <c r="B63">
+        <v>-0.11123622473963252</v>
+      </c>
+      <c r="C63">
+        <v>20.000224550651605</v>
+      </c>
+      <c r="D63">
+        <v>0.9971037467258795</v>
+      </c>
+      <c r="E63">
+        <v>0.0014392223251829242</v>
+      </c>
+      <c r="F63">
+        <v>0.07619467747619808</v>
+      </c>
+      <c r="G63">
+        <v>-4.714947323579749e-5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64">
+        <v>7.128338332282285</v>
+      </c>
+      <c r="B64">
+        <v>-0.11216580433809419</v>
+      </c>
+      <c r="C64">
+        <v>20.000435331116933</v>
+      </c>
+      <c r="D64">
+        <v>0.9916963127556572</v>
+      </c>
+      <c r="E64">
+        <v>0.002264653586888631</v>
+      </c>
+      <c r="F64">
+        <v>-0.1285105668173512</v>
+      </c>
+      <c r="G64">
+        <v>-0.0004092269628447307</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65">
+        <v>7.165631027617243</v>
+      </c>
+      <c r="B65">
+        <v>-0.1128061961774246</v>
+      </c>
+      <c r="C65">
+        <v>20.000216837287994</v>
+      </c>
+      <c r="D65">
+        <v>0.9958425286427576</v>
+      </c>
+      <c r="E65">
+        <v>0.0015633667366981266</v>
+      </c>
+      <c r="F65">
+        <v>0.09105786997485553</v>
+      </c>
+      <c r="G65">
+        <v>3.4239997307514815e-6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66">
+        <v>7.203169476659154</v>
+      </c>
+      <c r="B66">
+        <v>-0.11366512608101727</v>
+      </c>
+      <c r="C66">
+        <v>20.000212429811075</v>
+      </c>
+      <c r="D66">
+        <v>0.9957878870383703</v>
+      </c>
+      <c r="E66">
+        <v>0.0020965831106308026</v>
+      </c>
+      <c r="F66">
+        <v>0.09164213454987816</v>
+      </c>
+      <c r="G66">
+        <v>3.4509241483850042e-6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67">
+        <v>7.244115053035866</v>
+      </c>
+      <c r="B67">
+        <v>-0.11431154569230392</v>
+      </c>
+      <c r="C67">
+        <v>20.00036242158547</v>
+      </c>
+      <c r="D67">
+        <v>0.9949912807021745</v>
+      </c>
+      <c r="E67">
+        <v>0.001577259004980717</v>
+      </c>
+      <c r="F67">
+        <v>0.09990835577192315</v>
+      </c>
+      <c r="G67">
+        <v>1.0803715648572592e-6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68">
+        <v>7.285269826542091</v>
+      </c>
+      <c r="B68">
+        <v>-0.11497037895023712</v>
+      </c>
+      <c r="C68">
+        <v>20.000374442913785</v>
+      </c>
+      <c r="D68">
+        <v>0.9949389814530258</v>
+      </c>
+      <c r="E68">
+        <v>0.0016076734359030509</v>
+      </c>
+      <c r="F68">
+        <v>0.10042645776022509</v>
+      </c>
+      <c r="G68">
+        <v>1.098099081103257e-6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69">
+        <v>7.326608154011361</v>
+      </c>
+      <c r="B69">
+        <v>-0.11562305832056895</v>
+      </c>
+      <c r="C69">
+        <v>20.00037556727214</v>
+      </c>
+      <c r="D69">
+        <v>0.9948937716160765</v>
+      </c>
+      <c r="E69">
+        <v>0.0015926321481555526</v>
+      </c>
+      <c r="F69">
+        <v>0.10087285487161936</v>
+      </c>
+      <c r="G69">
+        <v>1.1192451810981327e-6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70">
+        <v>7.369911157634886</v>
+      </c>
+      <c r="B70">
+        <v>-0.11655865739923982</v>
+      </c>
+      <c r="C70">
+        <v>20.00040818590383</v>
+      </c>
+      <c r="D70">
+        <v>0.9943968623985592</v>
+      </c>
+      <c r="E70">
+        <v>0.0022823776048050844</v>
+      </c>
+      <c r="F70">
+        <v>0.10563804048527997</v>
+      </c>
+      <c r="G70">
+        <v>1.2156812768974237e-6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71">
+        <v>7.411659729358689</v>
+      </c>
+      <c r="B71">
+        <v>-0.11721924752861007</v>
+      </c>
+      <c r="C71">
+        <v>20.000384854531386</v>
+      </c>
+      <c r="D71">
+        <v>0.9947919019693412</v>
+      </c>
+      <c r="E71">
+        <v>0.0016118827267008085</v>
+      </c>
+      <c r="F71">
+        <v>0.10187055162842892</v>
+      </c>
+      <c r="G71">
+        <v>1.1389374419392085e-6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72">
+        <v>7.4503854359016595</v>
+      </c>
+      <c r="B72">
+        <v>-0.11786416991234455</v>
+      </c>
+      <c r="C72">
+        <v>20.000228275789713</v>
+      </c>
+      <c r="D72">
+        <v>0.9955177767558472</v>
+      </c>
+      <c r="E72">
+        <v>0.001574073804071973</v>
+      </c>
+      <c r="F72">
+        <v>0.09453739804563248</v>
+      </c>
+      <c r="G72">
+        <v>3.6394882134551053e-6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73">
+        <v>7.4925342229974365</v>
+      </c>
+      <c r="B73">
+        <v>-0.11871939028420586</v>
+      </c>
+      <c r="C73">
+        <v>20.00038383351028</v>
+      </c>
+      <c r="D73">
+        <v>0.9946923064203308</v>
+      </c>
+      <c r="E73">
+        <v>0.0020864139097541007</v>
+      </c>
+      <c r="F73">
+        <v>0.10282827889760762</v>
+      </c>
+      <c r="G73">
+        <v>1.133020028616569e-6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74">
+        <v>7.534878061153688</v>
+      </c>
+      <c r="B74">
+        <v>-0.11939065536747992</v>
+      </c>
+      <c r="C74">
+        <v>20.00039461352284</v>
+      </c>
+      <c r="D74">
+        <v>0.9946428609821709</v>
+      </c>
+      <c r="E74">
+        <v>0.001637765413155243</v>
+      </c>
+      <c r="F74">
+        <v>0.10331268195099491</v>
+      </c>
+      <c r="G74">
+        <v>1.1626231646255765e-6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75">
+        <v>7.577426231407261</v>
+      </c>
+      <c r="B75">
+        <v>-0.12006516618662696</v>
+      </c>
+      <c r="C75">
+        <v>20.000395248142087</v>
+      </c>
+      <c r="D75">
+        <v>0.9945910543122229</v>
+      </c>
+      <c r="E75">
+        <v>0.0016456523696332386</v>
+      </c>
+      <c r="F75">
+        <v>0.10380924832927282</v>
+      </c>
+      <c r="G75">
+        <v>1.1887224633417554e-6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76">
+        <v>7.620178848591056</v>
+      </c>
+      <c r="B76">
+        <v>-0.12074292145964519</v>
+      </c>
+      <c r="C76">
+        <v>20.000399308469895</v>
+      </c>
+      <c r="D76">
+        <v>0.9945390716203699</v>
+      </c>
+      <c r="E76">
+        <v>0.0016535206607317975</v>
+      </c>
+      <c r="F76">
+        <v>0.10430506446843828</v>
+      </c>
+      <c r="G76">
+        <v>1.196905388877891e-6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77">
+        <v>7.661376374449138</v>
+      </c>
+      <c r="B77">
+        <v>-0.12142577081832745</v>
+      </c>
+      <c r="C77">
+        <v>20.000374548748066</v>
+      </c>
+      <c r="D77">
+        <v>0.9949281133121204</v>
+      </c>
+      <c r="E77">
+        <v>0.0016663136206271673</v>
+      </c>
+      <c r="F77">
+        <v>0.1005329488429764</v>
+      </c>
+      <c r="G77">
+        <v>1.1134349045737627e-6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78">
+        <v>7.70119312863931</v>
+      </c>
+      <c r="B78">
+        <v>-0.12209819564134615</v>
+      </c>
+      <c r="C78">
+        <v>20.00026485651765</v>
+      </c>
+      <c r="D78">
+        <v>0.9952618158985411</v>
+      </c>
+      <c r="E78">
+        <v>0.0016411912534067547</v>
+      </c>
+      <c r="F78">
+        <v>0.09718507110858711</v>
+      </c>
+      <c r="G78">
+        <v>7.783596317207319e-7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79">
+        <v>7.744545841948116</v>
+      </c>
+      <c r="B79">
+        <v>-0.12278587402349075</v>
+      </c>
+      <c r="C79">
+        <v>20.000404741037382</v>
+      </c>
+      <c r="D79">
+        <v>0.9943861143908788</v>
+      </c>
+      <c r="E79">
+        <v>0.0016774296214994721</v>
+      </c>
+      <c r="F79">
+        <v>0.10575031044389907</v>
+      </c>
+      <c r="G79">
+        <v>1.2097488314605407e-6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80">
+        <v>7.788096834530364</v>
+      </c>
+      <c r="B80">
+        <v>-0.12347670323279877</v>
+      </c>
+      <c r="C80">
+        <v>20.00041267914357</v>
+      </c>
+      <c r="D80">
+        <v>0.9943336370480222</v>
+      </c>
+      <c r="E80">
+        <v>0.001685236888369937</v>
+      </c>
+      <c r="F80">
+        <v>0.10624155529033734</v>
+      </c>
+      <c r="G80">
+        <v>1.2436080658119664e-6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81">
+        <v>7.831854040149032</v>
+      </c>
+      <c r="B81">
+        <v>-0.12417080705343163</v>
+      </c>
+      <c r="C81">
+        <v>20.000417251543418</v>
+      </c>
+      <c r="D81">
+        <v>0.9942799241922886</v>
+      </c>
+      <c r="E81">
+        <v>0.0016931836961382501</v>
+      </c>
+      <c r="F81">
+        <v>0.1067419872418195</v>
+      </c>
+      <c r="G81">
+        <v>1.2528442476949355e-6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82">
+        <v>7.86117476664199</v>
+      </c>
+      <c r="B82">
+        <v>-0.12484533934611647</v>
+      </c>
+      <c r="C82">
+        <v>20.00020854392931</v>
+      </c>
+      <c r="D82">
+        <v>0.9974386559111622</v>
+      </c>
+      <c r="E82">
+        <v>0.0016451019475059846</v>
+      </c>
+      <c r="F82">
+        <v>0.07165936374109391</v>
+      </c>
+      <c r="G82">
+        <v>-4.117561102857836e-5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83">
+        <v>7.905290883214833</v>
+      </c>
+      <c r="B83">
+        <v>-0.1255463193799094</v>
+      </c>
+      <c r="C83">
+        <v>20.00041325241802</v>
+      </c>
+      <c r="D83">
+        <v>0.9941876136042096</v>
+      </c>
+      <c r="E83">
+        <v>0.0017096202443126485</v>
+      </c>
+      <c r="F83">
+        <v>0.10759649937095257</v>
+      </c>
+      <c r="G83">
+        <v>1.2549995564599818e-6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84">
+        <v>7.949602311138106</v>
+      </c>
+      <c r="B84">
+        <v>-0.12625040730844966</v>
+      </c>
+      <c r="C84">
+        <v>20.00042572318785</v>
+      </c>
+      <c r="D84">
+        <v>0.9941344640966966</v>
+      </c>
+      <c r="E84">
+        <v>0.0017174016517742497</v>
+      </c>
+      <c r="F84">
+        <v>0.1080853756718342</v>
+      </c>
+      <c r="G84">
+        <v>1.2888564118619507e-6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85">
+        <v>7.994121423143115</v>
+      </c>
+      <c r="B85">
+        <v>-0.12695779963464157</v>
+      </c>
+      <c r="C85">
+        <v>20.00042979841068</v>
+      </c>
+      <c r="D85">
+        <v>0.9940793900065391</v>
+      </c>
+      <c r="E85">
+        <v>0.0017254244282206707</v>
+      </c>
+      <c r="F85">
+        <v>0.10858961774049962</v>
+      </c>
+      <c r="G85">
+        <v>1.3024943072390505e-6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86">
+        <v>8.038849154790233</v>
+      </c>
+      <c r="B86">
+        <v>-0.12766851128117354</v>
+      </c>
+      <c r="C86">
+        <v>20.00043353748738</v>
+      </c>
+      <c r="D86">
+        <v>0.9940238814471317</v>
+      </c>
+      <c r="E86">
+        <v>0.001733472384122232</v>
+      </c>
+      <c r="F86">
+        <v>0.10909544296440227</v>
+      </c>
+      <c r="G86">
+        <v>1.315318998587664e-6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87">
+        <v>8.083785736250654</v>
+      </c>
+      <c r="B87">
+        <v>-0.1283825452416133</v>
+      </c>
+      <c r="C87">
+        <v>20.00043814633116</v>
+      </c>
+      <c r="D87">
+        <v>0.993968062725938</v>
+      </c>
+      <c r="E87">
+        <v>0.0017415257444921824</v>
+      </c>
+      <c r="F87">
+        <v>0.1096016974834207</v>
+      </c>
+      <c r="G87">
+        <v>1.3244136550861427e-6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88">
+        <v>8.128931899203312</v>
+      </c>
+      <c r="B88">
+        <v>-0.12909991466048806</v>
+      </c>
+      <c r="C88">
+        <v>20.00044112069172</v>
+      </c>
+      <c r="D88">
+        <v>0.9939117704379707</v>
+      </c>
+      <c r="E88">
+        <v>0.001749612756568247</v>
+      </c>
+      <c r="F88">
+        <v>0.11010986239353494</v>
+      </c>
+      <c r="G88">
+        <v>1.3412525401820178e-6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89">
+        <v>8.174287356792856</v>
+      </c>
+      <c r="B89">
+        <v>-0.12982061209213408</v>
+      </c>
+      <c r="C89">
+        <v>20.00044751505142</v>
+      </c>
+      <c r="D89">
+        <v>0.9938553342011741</v>
+      </c>
+      <c r="E89">
+        <v>0.001757676010497563</v>
+      </c>
+      <c r="F89">
+        <v>0.1106169238250444</v>
+      </c>
+      <c r="G89">
+        <v>1.3428062948945325e-6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90">
+        <v>8.211422975880957</v>
+      </c>
+      <c r="B90">
+        <v>-0.13056143598191605</v>
+      </c>
+      <c r="C90">
+        <v>20.00021584185666</v>
+      </c>
+      <c r="D90">
+        <v>0.9958769360539376</v>
+      </c>
+      <c r="E90">
+        <v>0.0018086422945701537</v>
+      </c>
+      <c r="F90">
+        <v>0.09067671972206968</v>
+      </c>
+      <c r="G90">
+        <v>3.4081107650068207e-6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91">
+        <v>8.257175375487588</v>
+      </c>
+      <c r="B91">
+        <v>-0.13128928884789998</v>
+      </c>
+      <c r="C91">
+        <v>20.000444335776496</v>
+      </c>
+      <c r="D91">
+        <v>0.9937495998140775</v>
+      </c>
+      <c r="E91">
+        <v>0.0017747358396734618</v>
+      </c>
+      <c r="F91">
+        <v>0.11156062892217831</v>
+      </c>
+      <c r="G91">
+        <v>1.3417996259554428e-6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92">
+        <v>8.303124551273624</v>
+      </c>
+      <c r="B92">
+        <v>-0.13202027852396622</v>
+      </c>
+      <c r="C92">
+        <v>20.00045640926613</v>
+      </c>
+      <c r="D92">
+        <v>0.9936938112493621</v>
+      </c>
+      <c r="E92">
+        <v>0.0017826230066021196</v>
+      </c>
+      <c r="F92">
+        <v>0.11205529055223658</v>
+      </c>
+      <c r="G92">
+        <v>1.3866895635127456e-6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93">
+        <v>8.32871940393607</v>
+      </c>
+      <c r="B93">
+        <v>-0.13269992555887827</v>
+      </c>
+      <c r="C93">
+        <v>20.0001268687317</v>
+      </c>
+      <c r="D93">
+        <v>0.9980561956305817</v>
+      </c>
+      <c r="E93">
+        <v>0.0016435271720546933</v>
+      </c>
+      <c r="F93">
+        <v>0.06259131688196955</v>
+      </c>
+      <c r="G93">
+        <v>-0.0001454138794220857</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94">
+        <v>8.375018451258518</v>
+      </c>
+      <c r="B94">
+        <v>-0.13343800297156155</v>
+      </c>
+      <c r="C94">
+        <v>20.00044835829346</v>
+      </c>
+      <c r="D94">
+        <v>0.9936005547440991</v>
+      </c>
+      <c r="E94">
+        <v>0.0017994046147026138</v>
+      </c>
+      <c r="F94">
+        <v>0.11287724288535851</v>
+      </c>
+      <c r="G94">
+        <v>1.3735344381726002e-6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95">
+        <v>8.421508771708083</v>
+      </c>
+      <c r="B95">
+        <v>-0.13417913540908108</v>
+      </c>
+      <c r="C95">
+        <v>20.000465428238144</v>
+      </c>
+      <c r="D95">
+        <v>0.9935447722552428</v>
+      </c>
+      <c r="E95">
+        <v>0.0018072139622509397</v>
+      </c>
+      <c r="F95">
+        <v>0.11336599411119666</v>
+      </c>
+      <c r="G95">
+        <v>1.424384976655362e-6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96">
+        <v>8.468210179973347</v>
+      </c>
+      <c r="B96">
+        <v>-0.13492363700122526</v>
+      </c>
+      <c r="C96">
+        <v>20.000470960169416</v>
+      </c>
+      <c r="D96">
+        <v>0.993486036570533</v>
+      </c>
+      <c r="E96">
+        <v>0.0018153916074823008</v>
+      </c>
+      <c r="F96">
+        <v>0.11387833571360945</v>
+      </c>
+      <c r="G96">
+        <v>1.4353631116680663e-6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97">
+        <v>8.515124157920559</v>
+      </c>
+      <c r="B97">
+        <v>-0.13567153302497303</v>
+      </c>
+      <c r="C97">
+        <v>20.00047418653088</v>
+      </c>
+      <c r="D97">
+        <v>0.9934267155659351</v>
+      </c>
+      <c r="E97">
+        <v>0.001823616482874458</v>
+      </c>
+      <c r="F97">
+        <v>0.11439342493684655</v>
+      </c>
+      <c r="G97">
+        <v>1.453320745764427e-6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98">
+        <v>8.56225099378071</v>
+      </c>
+      <c r="B98">
+        <v>-0.136422827347588</v>
+      </c>
+      <c r="C98">
+        <v>20.000478261458078</v>
+      </c>
+      <c r="D98">
+        <v>0.9933670752930157</v>
+      </c>
+      <c r="E98">
+        <v>0.0018318461299891636</v>
+      </c>
+      <c r="F98">
+        <v>0.11490891279412416</v>
+      </c>
+      <c r="G98">
+        <v>1.4670577521726613e-6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99">
+        <v>8.609590563590233</v>
+      </c>
+      <c r="B99">
+        <v>-0.1371775164133943</v>
+      </c>
+      <c r="C99">
+        <v>20.000484289806078</v>
+      </c>
+      <c r="D99">
+        <v>0.993307209211588</v>
+      </c>
+      <c r="E99">
+        <v>0.0018400657740515994</v>
+      </c>
+      <c r="F99">
+        <v>0.11542398545822295</v>
+      </c>
+      <c r="G99">
+        <v>1.4726905902902035e-6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100">
+        <v>8.657143829796023</v>
+      </c>
+      <c r="B100">
+        <v>-0.13793561892772369</v>
+      </c>
+      <c r="C100">
+        <v>20.00048667250571</v>
+      </c>
+      <c r="D100">
+        <v>0.9932467561225055</v>
+      </c>
+      <c r="E100">
+        <v>0.001848335887300684</v>
+      </c>
+      <c r="F100">
+        <v>0.11594176553929182</v>
+      </c>
+      <c r="G100">
+        <v>1.495189354498543e-6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101">
+        <v>8.704910370171243</v>
+      </c>
+      <c r="B101">
+        <v>-0.13869712406104776</v>
+      </c>
+      <c r="C101">
+        <v>20.00049368738637</v>
+      </c>
+      <c r="D101">
+        <v>0.9931862255984698</v>
+      </c>
+      <c r="E101">
+        <v>0.0018565698420135194</v>
+      </c>
+      <c r="F101">
+        <v>0.11645783514232909</v>
+      </c>
+      <c r="G101">
+        <v>1.496542782585446e-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>